<commit_message>
change: MealStatusを変更（基本, unlocked, uncooked）
</commit_message>
<xml_diff>
--- a/dbInittool/excels/MealStatus.xlsx
+++ b/dbInittool/excels/MealStatus.xlsx
@@ -27,7 +27,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -38,6 +38,12 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -71,10 +77,10 @@
   </cellStyleXfs>
   <cellXfs count="4">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
@@ -400,15 +406,15 @@
         <v>1</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="23.25">
       <c r="A2" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2" s="2">
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="23.25">
       <c r="A3" s="2">
         <v>0</v>
       </c>
@@ -416,7 +422,7 @@
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="23.25">
       <c r="A4" s="2">
         <v>0</v>
       </c>
@@ -424,15 +430,15 @@
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="23.25">
       <c r="A5" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B5" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="17.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="23.25">
       <c r="A6" s="2">
         <v>0</v>
       </c>
@@ -440,7 +446,7 @@
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="23.25">
       <c r="A7" s="2">
         <v>0</v>
       </c>
@@ -448,7 +454,7 @@
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="23.25">
       <c r="A8" s="2">
         <v>0</v>
       </c>
@@ -456,7 +462,7 @@
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="23.25">
       <c r="A9" s="2">
         <v>0</v>
       </c>
@@ -464,51 +470,51 @@
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="23.25">
       <c r="A10" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B10" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="17.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="23.25">
       <c r="A11" s="2">
         <v>1</v>
       </c>
       <c r="B11" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="23.25">
+      <c r="A12" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="17.25">
-      <c r="A12" s="2">
-        <v>0</v>
-      </c>
       <c r="B12" s="2">
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="23.25">
       <c r="A13" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B13" s="2">
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="23.25">
       <c r="A14" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B14" s="2">
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="23.25">
       <c r="A15" s="2"/>
       <c r="B15" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="23.25">
       <c r="A16" s="2"/>
       <c r="B16" s="2"/>
     </row>

</xml_diff>